<commit_message>
Updated BOM (not complete)
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mp\Documents\GitHub\MotorTCD-1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSiderskiy\Documents\GitHub\MotorTCD-1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCC6055-C7A9-469D-8350-55E41DE768AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECA54CA-12BB-49DD-9F6B-F353A9CD86D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{AF6C7077-7324-405B-8491-1FC26821D493}"/>
+    <workbookView xWindow="2430" yWindow="-2565" windowWidth="8850" windowHeight="4590" xr2:uid="{AF6C7077-7324-405B-8491-1FC26821D493}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Part</t>
   </si>
   <si>
-    <t>No.</t>
-  </si>
-  <si>
     <t>Mfct.</t>
   </si>
   <si>
     <t>Qty.</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -57,18 +51,9 @@
     <t>Motor drive controller</t>
   </si>
   <si>
-    <t>Roll White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disolvable Material </t>
-  </si>
-  <si>
     <t>Ultimaker Material PLA Material White  2.85 mm</t>
   </si>
   <si>
-    <t>PVA Disolvable 2.85 mm</t>
-  </si>
-  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -87,15 +72,9 @@
     <t>26 AWG, For soldering, Blue</t>
   </si>
   <si>
-    <t>26 AWG, For soldering, Yellow</t>
-  </si>
-  <si>
     <t>26 AWG, For soldering, Black</t>
   </si>
   <si>
-    <t>26 AWG, For soldering, White</t>
-  </si>
-  <si>
     <t>3.3V regulator</t>
   </si>
   <si>
@@ -139,6 +118,93 @@
   </si>
   <si>
     <t>Joystick shield for adruino</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Makestore.com.au</t>
+  </si>
+  <si>
+    <t>Unit Price (AUD)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>PLA Roll (White)</t>
+  </si>
+  <si>
+    <t>imaginables.com.au</t>
+  </si>
+  <si>
+    <t>Ultimaker</t>
+  </si>
+  <si>
+    <t>Ultimaker PLA</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>UL Style 1430 (to solder on motor pads),  26AWG, 4 lead Color Code 1</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>Mfct No.</t>
+  </si>
+  <si>
+    <t>1430-26-1-0500-004-1-TS</t>
+  </si>
+  <si>
+    <t>Vendor Part No.</t>
+  </si>
+  <si>
+    <t>CN472R-25-ND</t>
+  </si>
+  <si>
+    <t>CN475G-25-ND</t>
+  </si>
+  <si>
+    <t>1430-26-1-0500-007-1-TS</t>
+  </si>
+  <si>
+    <t>CN473L-25-ND</t>
+  </si>
+  <si>
+    <t>1430-26-1-0500-005-1-TS</t>
+  </si>
+  <si>
+    <t>CN469B-25-ND</t>
+  </si>
+  <si>
+    <t>1430-26-1-0500-001-1-TS</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>AP3429A</t>
+  </si>
+  <si>
+    <t>ADA4711</t>
+  </si>
+  <si>
+    <t>core-electronics.com.au</t>
+  </si>
+  <si>
+    <t>3.3V Output 1.2A Max</t>
+  </si>
+  <si>
+    <t>AC to DC Power</t>
   </si>
 </sst>
 </file>
@@ -236,7 +302,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -244,6 +310,8 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -552,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,237 +628,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40731ECD-81CB-44DF-8C89-20836147E38D}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="77.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="G4" s="3">
+        <v>5.62</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>11.54</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>11.54</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>11.54</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>11.54</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
@@ -826,8 +1035,24 @@
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
     </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C064C592-00BF-4755-83B8-A1710B7A9291}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F9CE6763-92F0-48F4-A1B7-B6634D50DB8D}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{7BCCE937-B073-4BC2-9968-BEF6D40FC095}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{075C0742-D95C-471D-8514-2ED08F61A326}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{A4A3C833-19A4-4209-A6F3-49659287A53C}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{3244BA7D-51D6-4A6E-8397-3818D91D2CC8}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{B33A8999-B4C7-4F52-861C-16B5D76CA96F}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{3D750A4F-137F-4DC0-B439-3B793939B4D5}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{2915A89C-147F-4F59-8EBB-6775CFC79440}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{9AC2A44F-0135-4787-BD54-DC0BEE0882C7}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{E1D34C00-492F-4E3E-8229-F7F27E79A9A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removing extraneous files. Added demo video
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mp\Documents\GitHub\MotorTCD-1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSiderskiy\Documents\GitHub\MotorTCD_EMBC_2023\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E197259E-D403-4FB4-A4B5-9E32BF86FFC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD523238-221A-4EC5-836E-89E156FE9B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2436" yWindow="-2568" windowWidth="8856" windowHeight="4596" xr2:uid="{AF6C7077-7324-405B-8491-1FC26821D493}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{AF6C7077-7324-405B-8491-1FC26821D493}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>Part</t>
   </si>
@@ -99,9 +110,6 @@
     <t>Jumper wires for arduino(male,female, both)</t>
   </si>
   <si>
-    <t>Joystick shield for adruino</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -195,18 +203,9 @@
     <t>3V-12VDC  27W power supply(7 output plugs with USB outlet)</t>
   </si>
   <si>
-    <t>CE05629</t>
-  </si>
-  <si>
     <t>MP-3316</t>
   </si>
   <si>
-    <t>Uno R3</t>
-  </si>
-  <si>
-    <t> It has 14 digital input/output pins (of which 6 can be used as PWM outputs), 6 analogue inputs, a 16 MHz crystal oscillator, a USB connection, a power jack, an ICSP header, and a reset button.</t>
-  </si>
-  <si>
     <t>Switchmode Plugpack(AC to DC Power)</t>
   </si>
   <si>
@@ -264,18 +263,6 @@
     <t>120pcs Multicolored Dupont Wire 40pin Male to Female, 40pin Male to Male, 40pin Female to Female Breadboard Jumper Wires</t>
   </si>
   <si>
-    <t>The shield sits atop the Arduino and turns it into a simple controller</t>
-  </si>
-  <si>
-    <t>Funduino</t>
-  </si>
-  <si>
-    <t>PHI1001392</t>
-  </si>
-  <si>
-    <t>phippselectronics.com</t>
-  </si>
-  <si>
     <t> 5.5 X 2.1mm Female Plug to 2 pin Female Screw terminals adapter</t>
   </si>
   <si>
@@ -286,13 +273,29 @@
   </si>
   <si>
     <t>CGTime-00013</t>
+  </si>
+  <si>
+    <t>Arduino Uno R3</t>
+  </si>
+  <si>
+    <t>A000066</t>
+  </si>
+  <si>
+    <t>ARDUINO CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A000066 </t>
+  </si>
+  <si>
+    <t>Controls the Motors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -381,8 +384,8 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -691,7 +694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -699,11 +702,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40731ECD-81CB-44DF-8C89-20836147E38D}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -721,22 +722,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -744,8 +745,8 @@
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>35</v>
+      <c r="J1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -756,10 +757,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -777,16 +778,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -795,7 +796,7 @@
         <v>76.900000000000006</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H19" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H18" si="0">F3*G3</f>
         <v>76.900000000000006</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -807,13 +808,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -831,52 +832,49 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="3">
-        <v>11.54</v>
+      <c r="G5" s="7">
+        <v>35.85</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>11.54</v>
+        <f>F5*G5</f>
+        <v>35.85</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -889,27 +887,27 @@
         <v>11.54</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -922,27 +920,27 @@
         <v>11.54</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -955,97 +953,103 @@
         <v>11.54</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>7.6</v>
+        <v>11.54</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>7.6</v>
+        <v>11.54</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>38.15</v>
+        <v>7.6</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>38.15</v>
+        <v>7.6</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>16.899999999999999</v>
+        <v>38.15</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="I11" t="s">
-        <v>59</v>
+        <v>38.15</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1053,13 +1057,13 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1072,7 +1076,7 @@
         <v>11.95</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1080,13 +1084,13 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>15875</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1099,7 +1103,7 @@
         <v>16.48</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1107,13 +1111,13 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="7">
+        <v>63</v>
+      </c>
+      <c r="D14" s="6">
         <v>1161524</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1134,10 +1138,10 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1150,7 +1154,7 @@
         <v>28.88</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1158,13 +1162,13 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1177,7 +1181,7 @@
         <v>9.9600000000000009</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1185,13 +1189,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1204,65 +1208,41 @@
         <v>13.86</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>13.95</v>
+        <v>10.53</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="0"/>
-        <v>13.95</v>
+        <v>10.53</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>10.53</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>10.53</v>
-      </c>
-      <c r="I19" t="s">
-        <v>83</v>
-      </c>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -1320,36 +1300,32 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{C064C592-00BF-4755-83B8-A1710B7A9291}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{F9CE6763-92F0-48F4-A1B7-B6634D50DB8D}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{7BCCE937-B073-4BC2-9968-BEF6D40FC095}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{075C0742-D95C-471D-8514-2ED08F61A326}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{A4A3C833-19A4-4209-A6F3-49659287A53C}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{3244BA7D-51D6-4A6E-8397-3818D91D2CC8}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{B33A8999-B4C7-4F52-861C-16B5D76CA96F}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{3D750A4F-137F-4DC0-B439-3B793939B4D5}"/>
-    <hyperlink ref="E6" r:id="rId9" xr:uid="{2915A89C-147F-4F59-8EBB-6775CFC79440}"/>
-    <hyperlink ref="E7" r:id="rId10" xr:uid="{9AC2A44F-0135-4787-BD54-DC0BEE0882C7}"/>
-    <hyperlink ref="E8" r:id="rId11" xr:uid="{E1D34C00-492F-4E3E-8229-F7F27E79A9A6}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{B5C8CC14-270A-46E5-9D3C-27368F1B5157}"/>
-    <hyperlink ref="E11" r:id="rId13" xr:uid="{485DF123-62EA-4AAF-90B3-8D6204CBDE6C}"/>
-    <hyperlink ref="E12" r:id="rId14" xr:uid="{148B7452-19F6-4D49-9837-AC09099909F7}"/>
-    <hyperlink ref="E13" r:id="rId15" xr:uid="{97837B5C-D688-484F-87D2-A9A3921B65FC}"/>
-    <hyperlink ref="E14" r:id="rId16" xr:uid="{6D49E9BD-B53A-4E17-95A1-EE81FE4AF553}"/>
-    <hyperlink ref="E15" r:id="rId17" xr:uid="{26BAFE4B-7F48-4754-A600-46BFCAA9B06F}"/>
-    <hyperlink ref="E16" r:id="rId18" xr:uid="{AB127230-822B-49D7-9C7B-BD8A6F12117C}"/>
-    <hyperlink ref="E17" r:id="rId19" xr:uid="{CE8F9CF0-37AA-433B-B808-7328808438A9}"/>
-    <hyperlink ref="E18" r:id="rId20" xr:uid="{F8317691-8568-4F96-B8A0-7CDFEA52FAF9}"/>
-    <hyperlink ref="E19" r:id="rId21" xr:uid="{0D187AB9-DDC5-4B12-BF87-4E5F4256F30E}"/>
-    <hyperlink ref="E9" r:id="rId22" xr:uid="{5013D8F8-9072-44C9-AAF0-0163B77ADF65}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{075C0742-D95C-471D-8514-2ED08F61A326}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{A4A3C833-19A4-4209-A6F3-49659287A53C}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{3244BA7D-51D6-4A6E-8397-3818D91D2CC8}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{B33A8999-B4C7-4F52-861C-16B5D76CA96F}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{3D750A4F-137F-4DC0-B439-3B793939B4D5}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{2915A89C-147F-4F59-8EBB-6775CFC79440}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{9AC2A44F-0135-4787-BD54-DC0BEE0882C7}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{E1D34C00-492F-4E3E-8229-F7F27E79A9A6}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{B5C8CC14-270A-46E5-9D3C-27368F1B5157}"/>
+    <hyperlink ref="E12" r:id="rId13" xr:uid="{148B7452-19F6-4D49-9837-AC09099909F7}"/>
+    <hyperlink ref="E13" r:id="rId14" xr:uid="{97837B5C-D688-484F-87D2-A9A3921B65FC}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{6D49E9BD-B53A-4E17-95A1-EE81FE4AF553}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{26BAFE4B-7F48-4754-A600-46BFCAA9B06F}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{AB127230-822B-49D7-9C7B-BD8A6F12117C}"/>
+    <hyperlink ref="E17" r:id="rId18" xr:uid="{CE8F9CF0-37AA-433B-B808-7328808438A9}"/>
+    <hyperlink ref="E18" r:id="rId19" xr:uid="{0D187AB9-DDC5-4B12-BF87-4E5F4256F30E}"/>
+    <hyperlink ref="E10" r:id="rId20" xr:uid="{5013D8F8-9072-44C9-AAF0-0163B77ADF65}"/>
+    <hyperlink ref="E5" r:id="rId21" xr:uid="{AF584F30-3F4B-40A8-A58C-280B6F3F18D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>